<commit_message>
Bigger networks seem to work now.
</commit_message>
<xml_diff>
--- a/tournament_results.xlsx
+++ b/tournament_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z27"/>
+  <dimension ref="A1:AM39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,140 +434,202 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>11</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>13</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>17</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>19</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>21</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>23</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>24</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>26</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>28</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>30</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>32</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>34</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>36</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>38</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>40</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>42</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>44</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>46</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>48</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>50</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>74</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="B2" t="n">
         <v>1</v>
@@ -585,10 +647,10 @@
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I2" t="n">
         <v>1</v>
@@ -615,10 +677,10 @@
         <v>1</v>
       </c>
       <c r="Q2" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="R2" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="S2" t="n">
         <v>1</v>
@@ -642,12 +704,53 @@
         <v>1</v>
       </c>
       <c r="Z2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -722,18 +825,59 @@
         <v>1</v>
       </c>
       <c r="Z3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>-1</v>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="B4" t="n">
         <v>-1</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
@@ -751,10 +895,10 @@
         <v>1</v>
       </c>
       <c r="I4" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K4" t="n">
         <v>1</v>
@@ -763,10 +907,10 @@
         <v>1</v>
       </c>
       <c r="M4" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="N4" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="O4" t="n">
         <v>1</v>
@@ -778,13 +922,13 @@
         <v>1</v>
       </c>
       <c r="R4" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="S4" t="n">
         <v>-1</v>
       </c>
       <c r="T4" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="U4" t="n">
         <v>1</v>
@@ -802,21 +946,62 @@
         <v>1</v>
       </c>
       <c r="Z4" t="n">
-        <v>-1</v>
+        <v>1</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>1</v>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="B5" t="n">
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
@@ -825,10 +1010,10 @@
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I5" t="n">
         <v>1</v>
@@ -882,12 +1067,53 @@
         <v>1</v>
       </c>
       <c r="Z5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>1</v>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
       <c r="B6" t="n">
         <v>1</v>
@@ -962,12 +1188,53 @@
         <v>1</v>
       </c>
       <c r="Z6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>1</v>
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="B7" t="n">
         <v>1</v>
@@ -979,10 +1246,10 @@
         <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
@@ -1024,10 +1291,10 @@
         <v>1</v>
       </c>
       <c r="T7" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="U7" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="V7" t="n">
         <v>1</v>
@@ -1042,12 +1309,53 @@
         <v>1</v>
       </c>
       <c r="Z7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>1</v>
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -1122,12 +1430,53 @@
         <v>1</v>
       </c>
       <c r="Z8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM8" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>1</v>
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
       </c>
       <c r="B9" t="n">
         <v>1</v>
@@ -1139,10 +1488,10 @@
         <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>
@@ -1202,12 +1551,53 @@
         <v>1</v>
       </c>
       <c r="Z9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM9" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>1</v>
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
       </c>
       <c r="B10" t="n">
         <v>1</v>
@@ -1225,10 +1615,10 @@
         <v>1</v>
       </c>
       <c r="G10" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I10" t="n">
         <v>1</v>
@@ -1240,10 +1630,10 @@
         <v>1</v>
       </c>
       <c r="L10" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="M10" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="N10" t="n">
         <v>1</v>
@@ -1258,10 +1648,10 @@
         <v>1</v>
       </c>
       <c r="R10" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="S10" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="T10" t="n">
         <v>1</v>
@@ -1270,10 +1660,10 @@
         <v>1</v>
       </c>
       <c r="V10" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="W10" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="X10" t="n">
         <v>1</v>
@@ -1282,12 +1672,53 @@
         <v>1</v>
       </c>
       <c r="Z10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM10" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>1</v>
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
       </c>
       <c r="B11" t="n">
         <v>1</v>
@@ -1305,10 +1736,10 @@
         <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H11" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I11" t="n">
         <v>1</v>
@@ -1362,12 +1793,53 @@
         <v>1</v>
       </c>
       <c r="Z11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>1</v>
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
       <c r="B12" t="n">
         <v>1</v>
@@ -1403,10 +1875,10 @@
         <v>1</v>
       </c>
       <c r="M12" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="N12" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="O12" t="n">
         <v>1</v>
@@ -1442,12 +1914,53 @@
         <v>1</v>
       </c>
       <c r="Z12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM12" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>1</v>
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
       </c>
       <c r="B13" t="n">
         <v>1</v>
@@ -1471,10 +1984,10 @@
         <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="J13" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K13" t="n">
         <v>1</v>
@@ -1522,12 +2035,53 @@
         <v>1</v>
       </c>
       <c r="Z13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AH13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM13" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>1</v>
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B14" t="n">
         <v>1</v>
@@ -1548,7 +2102,7 @@
         <v>1</v>
       </c>
       <c r="H14" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I14" t="n">
         <v>-1</v>
@@ -1557,7 +2111,7 @@
         <v>-1</v>
       </c>
       <c r="K14" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="L14" t="n">
         <v>1</v>
@@ -1603,11 +2157,52 @@
       </c>
       <c r="Z14" t="n">
         <v>1</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI14" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AJ14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM14" t="n">
+        <v>-1</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>1</v>
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
       </c>
       <c r="B15" t="n">
         <v>1</v>
@@ -1682,12 +2277,53 @@
         <v>1</v>
       </c>
       <c r="Z15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM15" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>1</v>
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="B16" t="n">
         <v>1</v>
@@ -1705,19 +2341,19 @@
         <v>1</v>
       </c>
       <c r="G16" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H16" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I16" t="n">
         <v>1</v>
       </c>
       <c r="J16" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="K16" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="L16" t="n">
         <v>1</v>
@@ -1763,17 +2399,58 @@
       </c>
       <c r="Z16" t="n">
         <v>1</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG16" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AH16" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AI16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM16" t="n">
+        <v>-1</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>1</v>
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
       </c>
       <c r="B17" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D17" t="n">
         <v>1</v>
@@ -1803,22 +2480,22 @@
         <v>1</v>
       </c>
       <c r="M17" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="N17" t="n">
         <v>-1</v>
       </c>
       <c r="O17" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="P17" t="n">
         <v>1</v>
       </c>
       <c r="Q17" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="R17" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="S17" t="n">
         <v>1</v>
@@ -1836,18 +2513,59 @@
         <v>1</v>
       </c>
       <c r="X17" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y17" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Z17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM17" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>1</v>
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
       </c>
       <c r="B18" t="n">
         <v>1</v>
@@ -1859,10 +2577,10 @@
         <v>1</v>
       </c>
       <c r="E18" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G18" t="n">
         <v>1</v>
@@ -1889,10 +2607,10 @@
         <v>1</v>
       </c>
       <c r="O18" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="P18" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Q18" t="n">
         <v>1</v>
@@ -1913,21 +2631,62 @@
         <v>1</v>
       </c>
       <c r="W18" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X18" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y18" t="n">
         <v>1</v>
       </c>
       <c r="Z18" t="n">
-        <v>-1</v>
+        <v>1</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM18" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>1</v>
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
       </c>
       <c r="B19" t="n">
         <v>1</v>
@@ -1936,10 +2695,10 @@
         <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F19" t="n">
         <v>1</v>
@@ -1948,10 +2707,10 @@
         <v>1</v>
       </c>
       <c r="H19" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="J19" t="n">
         <v>1</v>
@@ -1975,10 +2734,10 @@
         <v>1</v>
       </c>
       <c r="Q19" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="R19" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="S19" t="n">
         <v>1</v>
@@ -2002,12 +2761,53 @@
         <v>1</v>
       </c>
       <c r="Z19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM19" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>1</v>
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
       </c>
       <c r="B20" t="n">
         <v>1</v>
@@ -2082,12 +2882,53 @@
         <v>1</v>
       </c>
       <c r="Z20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD20" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AE20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM20" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
-        <v>1</v>
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
       </c>
       <c r="B21" t="n">
         <v>1</v>
@@ -2111,10 +2952,10 @@
         <v>1</v>
       </c>
       <c r="I21" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="J21" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K21" t="n">
         <v>1</v>
@@ -2129,7 +2970,7 @@
         <v>1</v>
       </c>
       <c r="O21" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="P21" t="n">
         <v>-1</v>
@@ -2138,16 +2979,16 @@
         <v>-1</v>
       </c>
       <c r="R21" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="S21" t="n">
         <v>1</v>
       </c>
       <c r="T21" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="U21" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="V21" t="n">
         <v>1</v>
@@ -2156,18 +2997,59 @@
         <v>1</v>
       </c>
       <c r="X21" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y21" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Z21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG21" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AH21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK21" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AL21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM21" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
-        <v>1</v>
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
       </c>
       <c r="B22" t="n">
         <v>1</v>
@@ -2242,12 +3124,53 @@
         <v>1</v>
       </c>
       <c r="Z22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG22" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AH22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM22" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
-        <v>1</v>
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
       </c>
       <c r="B23" t="n">
         <v>1</v>
@@ -2268,10 +3191,10 @@
         <v>1</v>
       </c>
       <c r="H23" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="J23" t="n">
         <v>1</v>
@@ -2322,15 +3245,56 @@
         <v>1</v>
       </c>
       <c r="Z23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB23" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AC23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG23" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AH23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI23" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AJ23" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AK23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM23" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
-        <v>-1</v>
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C24" t="n">
         <v>1</v>
@@ -2351,13 +3315,13 @@
         <v>1</v>
       </c>
       <c r="I24" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="J24" t="n">
         <v>-1</v>
       </c>
       <c r="K24" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="L24" t="n">
         <v>1</v>
@@ -2402,21 +3366,62 @@
         <v>1</v>
       </c>
       <c r="Z24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI24" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AJ24" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AK24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM24" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
-        <v>1</v>
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
       </c>
       <c r="B25" t="n">
         <v>1</v>
       </c>
       <c r="C25" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D25" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E25" t="n">
         <v>1</v>
@@ -2482,12 +3487,53 @@
         <v>1</v>
       </c>
       <c r="Z25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG25" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AH25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM25" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
-        <v>1</v>
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
       </c>
       <c r="B26" t="n">
         <v>1</v>
@@ -2502,10 +3548,10 @@
         <v>1</v>
       </c>
       <c r="F26" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G26" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H26" t="n">
         <v>1</v>
@@ -2529,10 +3575,10 @@
         <v>1</v>
       </c>
       <c r="O26" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="P26" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Q26" t="n">
         <v>1</v>
@@ -2553,21 +3599,62 @@
         <v>1</v>
       </c>
       <c r="W26" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X26" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y26" t="n">
         <v>1</v>
       </c>
       <c r="Z26" t="n">
-        <v>-1</v>
+        <v>1</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AB26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK26" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AL26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM26" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
-        <v>1</v>
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
       </c>
       <c r="B27" t="n">
         <v>1</v>
@@ -2576,7 +3663,7 @@
         <v>1</v>
       </c>
       <c r="D27" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E27" t="n">
         <v>-1</v>
@@ -2585,7 +3672,7 @@
         <v>-1</v>
       </c>
       <c r="G27" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="H27" t="n">
         <v>1</v>
@@ -2603,10 +3690,10 @@
         <v>1</v>
       </c>
       <c r="M27" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="N27" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="O27" t="n">
         <v>1</v>
@@ -2642,6 +3729,1497 @@
         <v>1</v>
       </c>
       <c r="Z27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC27" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AD27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE27" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AF27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI27" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AJ27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1</v>
+      </c>
+      <c r="E28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F28" t="n">
+        <v>1</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H28" t="n">
+        <v>1</v>
+      </c>
+      <c r="I28" t="n">
+        <v>1</v>
+      </c>
+      <c r="J28" t="n">
+        <v>1</v>
+      </c>
+      <c r="K28" t="n">
+        <v>1</v>
+      </c>
+      <c r="L28" t="n">
+        <v>1</v>
+      </c>
+      <c r="M28" t="n">
+        <v>1</v>
+      </c>
+      <c r="N28" t="n">
+        <v>1</v>
+      </c>
+      <c r="O28" t="n">
+        <v>1</v>
+      </c>
+      <c r="P28" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>1</v>
+      </c>
+      <c r="R28" t="n">
+        <v>-1</v>
+      </c>
+      <c r="S28" t="n">
+        <v>1</v>
+      </c>
+      <c r="T28" t="n">
+        <v>1</v>
+      </c>
+      <c r="U28" t="n">
+        <v>1</v>
+      </c>
+      <c r="V28" t="n">
+        <v>1</v>
+      </c>
+      <c r="W28" t="n">
+        <v>1</v>
+      </c>
+      <c r="X28" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC28" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AD28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI28" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AJ28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM28" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F29" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1</v>
+      </c>
+      <c r="H29" t="n">
+        <v>1</v>
+      </c>
+      <c r="I29" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J29" t="n">
+        <v>1</v>
+      </c>
+      <c r="K29" t="n">
+        <v>1</v>
+      </c>
+      <c r="L29" t="n">
+        <v>1</v>
+      </c>
+      <c r="M29" t="n">
+        <v>1</v>
+      </c>
+      <c r="N29" t="n">
+        <v>1</v>
+      </c>
+      <c r="O29" t="n">
+        <v>1</v>
+      </c>
+      <c r="P29" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>1</v>
+      </c>
+      <c r="R29" t="n">
+        <v>1</v>
+      </c>
+      <c r="S29" t="n">
+        <v>1</v>
+      </c>
+      <c r="T29" t="n">
+        <v>1</v>
+      </c>
+      <c r="U29" t="n">
+        <v>1</v>
+      </c>
+      <c r="V29" t="n">
+        <v>1</v>
+      </c>
+      <c r="W29" t="n">
+        <v>1</v>
+      </c>
+      <c r="X29" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>-1</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI29" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AJ29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM29" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1</v>
+      </c>
+      <c r="H30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I30" t="n">
+        <v>1</v>
+      </c>
+      <c r="J30" t="n">
+        <v>1</v>
+      </c>
+      <c r="K30" t="n">
+        <v>1</v>
+      </c>
+      <c r="L30" t="n">
+        <v>1</v>
+      </c>
+      <c r="M30" t="n">
+        <v>1</v>
+      </c>
+      <c r="N30" t="n">
+        <v>1</v>
+      </c>
+      <c r="O30" t="n">
+        <v>1</v>
+      </c>
+      <c r="P30" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>1</v>
+      </c>
+      <c r="R30" t="n">
+        <v>1</v>
+      </c>
+      <c r="S30" t="n">
+        <v>1</v>
+      </c>
+      <c r="T30" t="n">
+        <v>1</v>
+      </c>
+      <c r="U30" t="n">
+        <v>1</v>
+      </c>
+      <c r="V30" t="n">
+        <v>1</v>
+      </c>
+      <c r="W30" t="n">
+        <v>1</v>
+      </c>
+      <c r="X30" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AB30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI30" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AJ30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1</v>
+      </c>
+      <c r="F31" t="n">
+        <v>1</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1</v>
+      </c>
+      <c r="H31" t="n">
+        <v>1</v>
+      </c>
+      <c r="I31" t="n">
+        <v>1</v>
+      </c>
+      <c r="J31" t="n">
+        <v>1</v>
+      </c>
+      <c r="K31" t="n">
+        <v>1</v>
+      </c>
+      <c r="L31" t="n">
+        <v>1</v>
+      </c>
+      <c r="M31" t="n">
+        <v>1</v>
+      </c>
+      <c r="N31" t="n">
+        <v>1</v>
+      </c>
+      <c r="O31" t="n">
+        <v>1</v>
+      </c>
+      <c r="P31" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>1</v>
+      </c>
+      <c r="R31" t="n">
+        <v>1</v>
+      </c>
+      <c r="S31" t="n">
+        <v>1</v>
+      </c>
+      <c r="T31" t="n">
+        <v>1</v>
+      </c>
+      <c r="U31" t="n">
+        <v>1</v>
+      </c>
+      <c r="V31" t="n">
+        <v>1</v>
+      </c>
+      <c r="W31" t="n">
+        <v>1</v>
+      </c>
+      <c r="X31" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD31" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AE31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM31" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" t="n">
+        <v>1</v>
+      </c>
+      <c r="F32" t="n">
+        <v>1</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1</v>
+      </c>
+      <c r="I32" t="n">
+        <v>1</v>
+      </c>
+      <c r="J32" t="n">
+        <v>1</v>
+      </c>
+      <c r="K32" t="n">
+        <v>1</v>
+      </c>
+      <c r="L32" t="n">
+        <v>1</v>
+      </c>
+      <c r="M32" t="n">
+        <v>1</v>
+      </c>
+      <c r="N32" t="n">
+        <v>1</v>
+      </c>
+      <c r="O32" t="n">
+        <v>1</v>
+      </c>
+      <c r="P32" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>-1</v>
+      </c>
+      <c r="R32" t="n">
+        <v>1</v>
+      </c>
+      <c r="S32" t="n">
+        <v>1</v>
+      </c>
+      <c r="T32" t="n">
+        <v>1</v>
+      </c>
+      <c r="U32" t="n">
+        <v>1</v>
+      </c>
+      <c r="V32" t="n">
+        <v>1</v>
+      </c>
+      <c r="W32" t="n">
+        <v>1</v>
+      </c>
+      <c r="X32" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL32" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AM32" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" t="n">
+        <v>1</v>
+      </c>
+      <c r="F33" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1</v>
+      </c>
+      <c r="H33" t="n">
+        <v>1</v>
+      </c>
+      <c r="I33" t="n">
+        <v>1</v>
+      </c>
+      <c r="J33" t="n">
+        <v>1</v>
+      </c>
+      <c r="K33" t="n">
+        <v>1</v>
+      </c>
+      <c r="L33" t="n">
+        <v>1</v>
+      </c>
+      <c r="M33" t="n">
+        <v>1</v>
+      </c>
+      <c r="N33" t="n">
+        <v>1</v>
+      </c>
+      <c r="O33" t="n">
+        <v>1</v>
+      </c>
+      <c r="P33" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>1</v>
+      </c>
+      <c r="R33" t="n">
+        <v>1</v>
+      </c>
+      <c r="S33" t="n">
+        <v>1</v>
+      </c>
+      <c r="T33" t="n">
+        <v>1</v>
+      </c>
+      <c r="U33" t="n">
+        <v>1</v>
+      </c>
+      <c r="V33" t="n">
+        <v>1</v>
+      </c>
+      <c r="W33" t="n">
+        <v>1</v>
+      </c>
+      <c r="X33" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM33" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1</v>
+      </c>
+      <c r="F34" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1</v>
+      </c>
+      <c r="H34" t="n">
+        <v>1</v>
+      </c>
+      <c r="I34" t="n">
+        <v>1</v>
+      </c>
+      <c r="J34" t="n">
+        <v>1</v>
+      </c>
+      <c r="K34" t="n">
+        <v>1</v>
+      </c>
+      <c r="L34" t="n">
+        <v>1</v>
+      </c>
+      <c r="M34" t="n">
+        <v>1</v>
+      </c>
+      <c r="N34" t="n">
+        <v>1</v>
+      </c>
+      <c r="O34" t="n">
+        <v>1</v>
+      </c>
+      <c r="P34" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>1</v>
+      </c>
+      <c r="R34" t="n">
+        <v>1</v>
+      </c>
+      <c r="S34" t="n">
+        <v>1</v>
+      </c>
+      <c r="T34" t="n">
+        <v>1</v>
+      </c>
+      <c r="U34" t="n">
+        <v>1</v>
+      </c>
+      <c r="V34" t="n">
+        <v>1</v>
+      </c>
+      <c r="W34" t="n">
+        <v>1</v>
+      </c>
+      <c r="X34" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB34" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC34" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AD34" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AE34" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF34" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG34" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH34" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI34" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ34" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK34" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL34" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM34" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1</v>
+      </c>
+      <c r="F35" t="n">
+        <v>1</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1</v>
+      </c>
+      <c r="H35" t="n">
+        <v>1</v>
+      </c>
+      <c r="I35" t="n">
+        <v>1</v>
+      </c>
+      <c r="J35" t="n">
+        <v>1</v>
+      </c>
+      <c r="K35" t="n">
+        <v>1</v>
+      </c>
+      <c r="L35" t="n">
+        <v>1</v>
+      </c>
+      <c r="M35" t="n">
+        <v>1</v>
+      </c>
+      <c r="N35" t="n">
+        <v>1</v>
+      </c>
+      <c r="O35" t="n">
+        <v>1</v>
+      </c>
+      <c r="P35" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>1</v>
+      </c>
+      <c r="R35" t="n">
+        <v>1</v>
+      </c>
+      <c r="S35" t="n">
+        <v>1</v>
+      </c>
+      <c r="T35" t="n">
+        <v>1</v>
+      </c>
+      <c r="U35" t="n">
+        <v>1</v>
+      </c>
+      <c r="V35" t="n">
+        <v>1</v>
+      </c>
+      <c r="W35" t="n">
+        <v>1</v>
+      </c>
+      <c r="X35" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG35" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AH35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM35" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>69</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" t="n">
+        <v>1</v>
+      </c>
+      <c r="F36" t="n">
+        <v>1</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1</v>
+      </c>
+      <c r="H36" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I36" t="n">
+        <v>1</v>
+      </c>
+      <c r="J36" t="n">
+        <v>1</v>
+      </c>
+      <c r="K36" t="n">
+        <v>1</v>
+      </c>
+      <c r="L36" t="n">
+        <v>1</v>
+      </c>
+      <c r="M36" t="n">
+        <v>1</v>
+      </c>
+      <c r="N36" t="n">
+        <v>1</v>
+      </c>
+      <c r="O36" t="n">
+        <v>1</v>
+      </c>
+      <c r="P36" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>-1</v>
+      </c>
+      <c r="R36" t="n">
+        <v>1</v>
+      </c>
+      <c r="S36" t="n">
+        <v>1</v>
+      </c>
+      <c r="T36" t="n">
+        <v>-1</v>
+      </c>
+      <c r="U36" t="n">
+        <v>1</v>
+      </c>
+      <c r="V36" t="n">
+        <v>1</v>
+      </c>
+      <c r="W36" t="n">
+        <v>1</v>
+      </c>
+      <c r="X36" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y36" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z36" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA36" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB36" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC36" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD36" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE36" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF36" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG36" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AH36" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI36" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ36" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK36" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL36" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM36" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1</v>
+      </c>
+      <c r="F37" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G37" t="n">
+        <v>1</v>
+      </c>
+      <c r="H37" t="n">
+        <v>1</v>
+      </c>
+      <c r="I37" t="n">
+        <v>1</v>
+      </c>
+      <c r="J37" t="n">
+        <v>1</v>
+      </c>
+      <c r="K37" t="n">
+        <v>1</v>
+      </c>
+      <c r="L37" t="n">
+        <v>-1</v>
+      </c>
+      <c r="M37" t="n">
+        <v>-1</v>
+      </c>
+      <c r="N37" t="n">
+        <v>1</v>
+      </c>
+      <c r="O37" t="n">
+        <v>1</v>
+      </c>
+      <c r="P37" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>1</v>
+      </c>
+      <c r="R37" t="n">
+        <v>1</v>
+      </c>
+      <c r="S37" t="n">
+        <v>1</v>
+      </c>
+      <c r="T37" t="n">
+        <v>1</v>
+      </c>
+      <c r="U37" t="n">
+        <v>1</v>
+      </c>
+      <c r="V37" t="n">
+        <v>1</v>
+      </c>
+      <c r="W37" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X37" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y37" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE37" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AF37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F38" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G38" t="n">
+        <v>1</v>
+      </c>
+      <c r="H38" t="n">
+        <v>1</v>
+      </c>
+      <c r="I38" t="n">
+        <v>1</v>
+      </c>
+      <c r="J38" t="n">
+        <v>1</v>
+      </c>
+      <c r="K38" t="n">
+        <v>1</v>
+      </c>
+      <c r="L38" t="n">
+        <v>1</v>
+      </c>
+      <c r="M38" t="n">
+        <v>1</v>
+      </c>
+      <c r="N38" t="n">
+        <v>1</v>
+      </c>
+      <c r="O38" t="n">
+        <v>1</v>
+      </c>
+      <c r="P38" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>1</v>
+      </c>
+      <c r="R38" t="n">
+        <v>1</v>
+      </c>
+      <c r="S38" t="n">
+        <v>1</v>
+      </c>
+      <c r="T38" t="n">
+        <v>1</v>
+      </c>
+      <c r="U38" t="n">
+        <v>1</v>
+      </c>
+      <c r="V38" t="n">
+        <v>1</v>
+      </c>
+      <c r="W38" t="n">
+        <v>1</v>
+      </c>
+      <c r="X38" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y38" t="n">
+        <v>-1</v>
+      </c>
+      <c r="Z38" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA38" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB38" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AC38" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD38" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE38" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF38" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG38" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH38" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI38" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ38" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK38" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL38" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" t="n">
+        <v>1</v>
+      </c>
+      <c r="F39" t="n">
+        <v>1</v>
+      </c>
+      <c r="G39" t="n">
+        <v>1</v>
+      </c>
+      <c r="H39" t="n">
+        <v>1</v>
+      </c>
+      <c r="I39" t="n">
+        <v>1</v>
+      </c>
+      <c r="J39" t="n">
+        <v>1</v>
+      </c>
+      <c r="K39" t="n">
+        <v>1</v>
+      </c>
+      <c r="L39" t="n">
+        <v>1</v>
+      </c>
+      <c r="M39" t="n">
+        <v>1</v>
+      </c>
+      <c r="N39" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O39" t="n">
+        <v>-1</v>
+      </c>
+      <c r="P39" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>1</v>
+      </c>
+      <c r="R39" t="n">
+        <v>1</v>
+      </c>
+      <c r="S39" t="n">
+        <v>1</v>
+      </c>
+      <c r="T39" t="n">
+        <v>-1</v>
+      </c>
+      <c r="U39" t="n">
+        <v>1</v>
+      </c>
+      <c r="V39" t="n">
+        <v>1</v>
+      </c>
+      <c r="W39" t="n">
+        <v>1</v>
+      </c>
+      <c r="X39" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y39" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z39" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA39" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB39" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC39" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD39" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE39" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF39" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG39" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH39" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI39" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ39" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK39" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL39" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM39" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>